<commit_message>
Capítulo 6 y workflows
</commit_message>
<xml_diff>
--- a/DRE/cap06-Workflows/WF-Overhaul/IPT_ACRM_TablasDetalladaVentas_150521.xlsx
+++ b/DRE/cap06-Workflows/WF-Overhaul/IPT_ACRM_TablasDetalladaVentas_150521.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel Campos\Desktop\Documents\GitHub\Ingeteam\DRE\cap06-Workflows\WF-Overhaul\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Documents\GitHub\Ingeteam\DRE\cap06-Workflows\WF-Overhaul\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7605" tabRatio="919" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7605" tabRatio="919" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas_VTA.010" sheetId="3" r:id="rId1"/>
@@ -282,7 +282,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -414,96 +414,85 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,16 +777,18 @@
   <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,18 +797,18 @@
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>54</v>
       </c>
     </row>
@@ -831,111 +822,113 @@
   <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="25"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="7" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="7" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="15" t="s">
         <v>33</v>
       </c>
     </row>
@@ -956,91 +949,93 @@
   <dimension ref="B4:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:4" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:4" s="20" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D8"/>
+      <c r="D8" s="14"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D9"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D10"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D11"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D12"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D13"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D14"/>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D15"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D16"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18"/>
+      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19"/>
+      <c r="D19" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1048,6 +1043,7 @@
     <mergeCell ref="D4:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1055,17 +1051,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1074,138 +1070,138 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="24" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="25" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="25" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="25" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="25" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="25" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="25" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="25" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1219,219 +1215,221 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" style="8" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" style="26" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:4" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:4" s="20" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+    <row r="12" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="15" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="15" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="15" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1449,16 +1447,18 @@
   <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1467,34 +1467,34 @@
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1508,69 +1508,71 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1586,28 +1588,30 @@
   <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="14" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="15" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1620,43 +1624,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="14.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="14" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1672,68 +1678,70 @@
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="15" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>